<commit_message>
updated plots and code
</commit_message>
<xml_diff>
--- a/files/data/all trials - dichotomous outcomes.xlsx
+++ b/files/data/all trials - dichotomous outcomes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobba\Dropbox\work\z_research\OpenMetaAnalysis\Sepsis - fluid volume and timing\Manuscripts and abstracts\2023 - Mike fluid manuscript\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD354B2B-E775-42D1-9BF1-6471219C3969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847B7252-50B4-4BCA-AD09-59064816D375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23700" yWindow="3480" windowWidth="20475" windowHeight="11385" activeTab="1" xr2:uid="{1DD3E89D-2144-4D31-B3D0-EE59517C63B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{1DD3E89D-2144-4D31-B3D0-EE59517C63B2}"/>
   </bookViews>
   <sheets>
     <sheet name="all trials - sepsis fluids - di" sheetId="1" r:id="rId1"/>
@@ -685,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -718,18 +718,19 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1156,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7557B9D-92FE-40D8-BD27-FD33AAF73826}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,10 +1252,10 @@
         <v>45</v>
       </c>
       <c r="J2" s="10">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="K2" s="10">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>36</v>
@@ -1378,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C6EC73-315F-47D8-A518-B9E22CBB7F5A}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,26 +1395,26 @@
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="L1" s="15" t="s">
+      <c r="J1" s="17"/>
+      <c r="L1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1436,22 +1437,22 @@
       <c r="H2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1694,7 +1695,7 @@
         <f>E10+H10</f>
         <v>2219.3000000000002</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="18">
         <f>ROUND(I10/75,1)</f>
         <v>29.6</v>
       </c>
@@ -1958,7 +1959,7 @@
         <f>E19+H19</f>
         <v>3728.8</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="18">
         <f>ROUND(I19/75,1)</f>
         <v>49.7</v>
       </c>

</xml_diff>